<commit_message>
commit EXCEL with comments on variable renaming
</commit_message>
<xml_diff>
--- a/fields 3H-4C_comments_JH.xlsx
+++ b/fields 3H-4C_comments_JH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josch\Dropbox\Uniklinikum Heidelberg\Arbeit\Collaboration with Rukshana\ABCD4kids - SAP after 3rd meeting\final analysis dataset ABCD4kids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31304D38-5179-4EC2-98A1-9CB08CFD73C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755F4F73-D803-4196-8EE9-F9B13AB1AC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="550" xr2:uid="{C7F7ABEC-3494-4A9D-8744-1E7551F63558}"/>
+    <workbookView xWindow="40920" yWindow="3660" windowWidth="29040" windowHeight="15720" tabRatio="550" xr2:uid="{C7F7ABEC-3494-4A9D-8744-1E7551F63558}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="154">
   <si>
     <t>Variables in 4C</t>
   </si>
@@ -146,9 +146,6 @@
     <t>base_pwv_sds</t>
   </si>
   <si>
-    <t>pwv_sds_age</t>
-  </si>
-  <si>
     <t>echodate</t>
   </si>
   <si>
@@ -420,9 +417,6 @@
   </si>
   <si>
     <t xml:space="preserve">under_renal </t>
-  </si>
-  <si>
-    <t>pwd_sds_height</t>
   </si>
   <si>
     <t>additional fields to be added on</t>
@@ -481,10 +475,6 @@
     <t>ABCD4kids_analysis_group</t>
   </si>
   <si>
-    <t>Comments by Jonas on variable (category) label conversion
-before executing row-wise joining operation of 3H with 4C</t>
-  </si>
-  <si>
     <t>Variable "ethnicity" in 3H was renamed to "ethnic". Variable ethnic in 4C and 3H  was converted into a factor (categorical) variable with text category labels in line with 4C category label dictionary format.sasbdt.</t>
   </si>
   <si>
@@ -495,39 +485,6 @@
   </si>
   <si>
     <t>3H-to-4C variable label conversion applied</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">starting_date_hd 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(starting_date_hd  not used because of erroneous date entries; instead 3H variable dt_basevis was used -&gt; see comment for explanation)</t>
-    </r>
-  </si>
-  <si>
-    <t>New field "transplanted" added in 4C which indicates per included visit if the patient was already transplanted at that visit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newly created variable "ABCD4kids_analysis_group" added to overall joined analysis dataset which indicates each patient visit´s assigned analysis group </t>
-  </si>
-  <si>
-    <t>3H variable "base_pwv_sds" renamed to pwv_sds_age. SDS variable pws_sds_a in 4C newly calculated with lms-method.</t>
-  </si>
-  <si>
-    <t>pwd_sds_height newly calculated 
-with lms-method.</t>
-  </si>
-  <si>
-    <t>RWT and RWTa calculated in 4C based on 
-formulas shared by Priyanka. Lvh can be based on RWTa using cutoff value.</t>
   </si>
   <si>
     <r>
@@ -618,12 +575,127 @@
       <t xml:space="preserve"> = 0. Hence, at the moment of dt_basevis the patient was ~ initiating RRT.</t>
     </r>
   </si>
+  <si>
+    <t>pwv_sds_a</t>
+  </si>
+  <si>
+    <t>pwd_sds_h</t>
+  </si>
+  <si>
+    <t>pwd_sds_h newly calculated 
+with lms-method in 3H and 4C.</t>
+  </si>
+  <si>
+    <t>3H variable "base_pwv_sds" renamed to pwv_sds_a. SDS variable pws_sds_a newly calculated in 4C with lms-method.</t>
+  </si>
+  <si>
+    <t>RWT and RWTa calculated in 4C based on 
+formulas shared by Priyanka. Lvh can be calculated based on RWTa.</t>
+  </si>
+  <si>
+    <t>Additional Comments:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) In 3H, medication group variables only seem to represent when a patient was on a medication from a medication group (value: 1), but do not indicate when a patient was NOT on a medication from the medication group
+(value = 0 entries would be needed but are not available; only NA i.e. missing values are present).
+2) 3H variables mtho_Fesupp and mtho_epo are not  of binary type but take on different integer values from 0-4. Consistent interpretation of category levels must be established here. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Binary medication group variables formed in 4C which indicate if a patient is on at least one medication per medication group at a visit (value: 1), or currently not on any medication per medication group at a visit (value: 0).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3H-to-4C variable label conversion applied for medication groups. But there are still issues (see comments below).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3H-to-4C variable label conversion applied;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Is base_cimt in 3H really carotid artery IMT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>left</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (this is what the variable imtl represents in 4C)? </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">starting_date_hd 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(starting_date_hd  not used because of erroneous date entries; instead 3H variable dt_basevis was used -&gt; see comment for explanation)</t>
+    </r>
+  </si>
+  <si>
+    <t>Comments by Jonas on variable (category) label renaming/conversion before executing row-wise joining operation of 3H with 4C</t>
+  </si>
+  <si>
+    <t>New field "transplanted" added in 4C which indicates per included visit if the patient received a transplant before that visit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newly created variable "ABCD4kids_analysis_group" in joined analysis dataset indicates each patient visit´s assigned analysis group </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -661,16 +733,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -786,7 +883,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -825,15 +922,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -858,6 +946,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -867,17 +961,25 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1194,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FE33AC-25CD-453E-B997-C7AB32BCCE6F}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1203,10 +1305,10 @@
     <col min="1" max="1" width="55.9296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.19921875" customWidth="1"/>
-    <col min="4" max="4" width="38.06640625" customWidth="1"/>
+    <col min="4" max="4" width="44.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="26" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1214,10 +1316,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1228,7 +1330,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1239,7 +1341,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="6" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
@@ -1250,10 +1352,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="6" customFormat="1" ht="57" x14ac:dyDescent="0.45">
@@ -1264,10 +1366,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1278,7 +1380,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1289,7 +1391,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1300,7 +1402,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="6" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -1308,11 +1410,11 @@
         <v>14</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="11" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
@@ -1320,24 +1422,24 @@
         <v>15</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="6" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1348,7 +1450,7 @@
         <v>17</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1359,18 +1461,18 @@
         <v>19</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1381,7 +1483,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1392,7 +1494,7 @@
         <v>23</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1403,7 +1505,7 @@
         <v>25</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1414,18 +1516,19 @@
         <v>27</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="38" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>142</v>
+      <c r="C19" s="16"/>
+      <c r="D19" s="11" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1436,7 +1539,7 @@
         <v>31</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -1447,551 +1550,555 @@
         <v>34</v>
       </c>
       <c r="D21" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="24" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A22" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" s="27" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A22" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="40" t="s">
+      <c r="B23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D22" s="38" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>125</v>
-      </c>
       <c r="D23" s="8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="30"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="D25" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="6" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="6" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A26" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="42" t="s">
-        <v>133</v>
+      <c r="C26" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="D27" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="D28" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="D29" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="D30" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="D31" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="D32" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="D33" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="D34" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="D35" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D36" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="D37" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>65</v>
-      </c>
       <c r="D39" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="D40" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="D41" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>71</v>
-      </c>
       <c r="D42" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="D43" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A44" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>75</v>
-      </c>
       <c r="D44" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A45" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="D45" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="D46" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A47" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="D47" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A48" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>83</v>
-      </c>
       <c r="D48" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="D49" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="D50" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="29" t="s">
+      <c r="B51" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="24" t="s">
-        <v>89</v>
-      </c>
       <c r="D51" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A52" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="D52" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A53" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="D53" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="21" customFormat="1" ht="145.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" s="24" customFormat="1" ht="51.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="12" t="s">
+      <c r="B54" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B54" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>142</v>
+      <c r="C54" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" s="39" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="B55" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="36"/>
-      <c r="D55" s="19"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="40"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="C56" s="35"/>
+      <c r="D56" s="41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="171" x14ac:dyDescent="0.45">
+      <c r="A57" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C56" s="36"/>
-      <c r="D56" s="19"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A57" s="13" t="s">
+      <c r="B57" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B57" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="C57" s="36"/>
-      <c r="D57" s="19"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="42" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B58" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="B58" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="C58" s="36"/>
-      <c r="D58" s="19"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="40"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B59" s="32"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="19"/>
+        <v>103</v>
+      </c>
+      <c r="B59" s="29"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="40"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="B60" s="32"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="19"/>
+        <v>104</v>
+      </c>
+      <c r="B60" s="29"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="40"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B61" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C61" s="36"/>
-      <c r="D61" s="19"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="40"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="B62" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="C62" s="36"/>
-      <c r="D62" s="19"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="40"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="B63" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="C63" s="36"/>
-      <c r="D63" s="19"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="40"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B64" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B64" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="C64" s="36"/>
-      <c r="D64" s="19"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="40"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="B65" s="33"/>
-      <c r="C65" s="36"/>
-      <c r="D65" s="19"/>
+        <v>113</v>
+      </c>
+      <c r="B65" s="30"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="40"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B66" s="33"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="19"/>
+        <v>114</v>
+      </c>
+      <c r="B66" s="30"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="40"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B67" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="C67" s="36"/>
-      <c r="D67" s="19"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="40"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B68" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B68" s="32" t="s">
+      <c r="C68" s="35"/>
+      <c r="D68" s="40"/>
+    </row>
+    <row r="69" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C68" s="36"/>
-      <c r="D68" s="19"/>
-    </row>
-    <row r="69" spans="1:4" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B69" s="34"/>
-      <c r="C69" s="37"/>
-      <c r="D69" s="20"/>
+      <c r="B69" s="31"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="43"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A72" s="20" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A72" s="23" t="s">
-        <v>131</v>
-      </c>
       <c r="B72" t="s">
-        <v>130</v>
-      </c>
-      <c r="D72" s="21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="57" x14ac:dyDescent="0.45">
-      <c r="A73" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="B73" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C73" s="25"/>
-      <c r="D73" s="22" t="s">
-        <v>145</v>
+        <v>128</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A73" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B73" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="22"/>
+      <c r="D73" s="19" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>